<commit_message>
tracker sheet with label complete
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_Srividhya.xlsx
+++ b/Wave 5_React_Tracker_Srividhya.xlsx
@@ -407,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,7 +418,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,10 +509,10 @@
         <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
commited gmail compose component code
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_Srividhya.xlsx
+++ b/Wave 5_React_Tracker_Srividhya.xlsx
@@ -407,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -512,10 +512,10 @@
         <v>14</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
commited with gmail view
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_Srividhya.xlsx
+++ b/Wave 5_React_Tracker_Srividhya.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Inbox Mails</t>
-  </si>
-  <si>
-    <t>In-Progress</t>
   </si>
   <si>
     <t>TODO</t>
@@ -407,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,7 +415,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -515,13 +512,13 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>